<commit_message>
Interface do software pronta, lógica matemática ainda com alguns erros
</commit_message>
<xml_diff>
--- a/Desktop/Projeto_Producao/relatorio_solver.xlsx
+++ b/Desktop/Projeto_Producao/relatorio_solver.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,31 +448,91 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>x1</t>
+          <t>s1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.3333333</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>x2</t>
+          <t>s2</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.3333333</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Função Objetivo</t>
+          <t>s3</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12.6666665</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>s4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>x2</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>x3</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>x4</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Z (Função Objetivo)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>97600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>